<commit_message>
add styles and custom
</commit_message>
<xml_diff>
--- a/planning/TestStyles.xlsx
+++ b/planning/TestStyles.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Style de base</t>
   </si>
   <si>
+    <t>Style bold</t>
+  </si>
+  <si>
     <t>Style CM</t>
   </si>
   <si>
@@ -24,6 +27,18 @@
   </si>
   <si>
     <t>Style TP</t>
+  </si>
+  <si>
+    <t>Style CC</t>
+  </si>
+  <si>
+    <t>Style Week Num</t>
+  </si>
+  <si>
+    <t>Style Date</t>
+  </si>
+  <si>
+    <t>Style Holiday</t>
   </si>
 </sst>
 </file>
@@ -31,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -48,6 +63,32 @@
       <name val="Arial"/>
       <sz val="12.0"/>
       <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -60,7 +101,7 @@
       <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,32 +110,72 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="15"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="5"/>
+        <fgColor rgb="2196F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="2196F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="8BC34A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="8BC34A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC107"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC107"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F44336"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F44336"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E0E0E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E0E0E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="BDBDBD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="BDBDBD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF5722"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5722"/>
       </patternFill>
     </fill>
   </fills>
@@ -110,18 +191,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -130,33 +226,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="18.75" customWidth="true"/>
+    <col min="3" max="3" width="18.75" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="24.0" customHeight="true">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
+      <c r="C1" t="s" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="24.0" customHeight="true">
-      <c r="A2" t="s" s="2">
-        <v>1</v>
+      <c r="A2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="24.0" customHeight="true">
-      <c r="A3" t="s" s="3">
-        <v>2</v>
+      <c r="A3" t="s" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s" s="7">
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="24.0" customHeight="true">
-      <c r="A4" t="s" s="4">
-        <v>3</v>
+      <c r="A4" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" ht="24.0" customHeight="true">
+      <c r="A5" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add merge and border
</commit_message>
<xml_diff>
--- a/planning/TestStyles.xlsx
+++ b/planning/TestStyles.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Style de base</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Style Holiday</t>
+  </si>
+  <si>
+    <t>merged</t>
   </si>
 </sst>
 </file>
@@ -46,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -100,6 +103,11 @@
       <sz val="12.0"/>
       <color indexed="8"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -179,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -187,11 +195,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="double"/>
+    </border>
+    <border>
+      <top style="double"/>
+      <bottom style="double"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
@@ -218,6 +233,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -226,7 +244,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -273,7 +291,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" s="10" customFormat="true"/>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>